<commit_message>
added ethanol tap off descriptions and work on documenting ignition sequence
</commit_message>
<xml_diff>
--- a/Avionics/EngineControlUnit-Firmware/Control-Module/engine tasks.xlsx
+++ b/Avionics/EngineControlUnit-Firmware/Control-Module/engine tasks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/EngineControlUnit-Firmware/Control-Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3069FB3C-A975-624C-B175-DDE7C8AD7C7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA1E056-8FE2-7644-99A6-CC7EAE204EFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="27240" windowHeight="16280" xr2:uid="{504D1F5D-43FB-1F42-833A-C8ADE7C72FF6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Checks" sheetId="1" r:id="rId1"/>
+    <sheet name="IGN-Sequence" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Engine Tasks</t>
   </si>
@@ -57,9 +58,6 @@
     <t>Engine Purge Task</t>
   </si>
   <si>
-    <t>Enginr Chill Task</t>
-  </si>
-  <si>
     <t>Verify operation of valve suite in engine feed systems. Valve such as</t>
   </si>
   <si>
@@ -70,13 +68,46 @@
   </si>
   <si>
     <t>load cells</t>
+  </si>
+  <si>
+    <t>Ignition Sequence</t>
+  </si>
+  <si>
+    <t>Engine Chill Task</t>
+  </si>
+  <si>
+    <t>Entry Checks</t>
+  </si>
+  <si>
+    <t>Sequence Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          v</t>
+  </si>
+  <si>
+    <t>Boot into safe mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel and Oxidizer lines are flushed with nitrogen gas to remove residue </t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Custom Operation</t>
+  </si>
+  <si>
+    <t>Start Engine Purge Task</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +126,18 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -131,6 +174,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4343CAA3-B634-E940-93C4-706CF3EA40E8}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G15"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,166 +516,325 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="H4" s="3" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
       <c r="O4" s="5"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
+  <mergeCells count="18">
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
     <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
     <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AE33BC-5252-A44F-9B39-E4146C0908FC}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
documentation additions with incremental firmware changes
</commit_message>
<xml_diff>
--- a/Avionics/EngineControlUnit-Firmware/Control-Module/engine tasks.xlsx
+++ b/Avionics/EngineControlUnit-Firmware/Control-Module/engine tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/EngineControlUnit-Firmware/Control-Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA1E056-8FE2-7644-99A6-CC7EAE204EFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F354D887-4040-B249-8B3E-BEEFCFAA894F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="27240" windowHeight="16280" xr2:uid="{504D1F5D-43FB-1F42-833A-C8ADE7C72FF6}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="27240" windowHeight="16280" activeTab="1" xr2:uid="{504D1F5D-43FB-1F42-833A-C8ADE7C72FF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Checks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Engine Tasks</t>
   </si>
@@ -70,9 +70,6 @@
     <t>load cells</t>
   </si>
   <si>
-    <t>Ignition Sequence</t>
-  </si>
-  <si>
     <t>Engine Chill Task</t>
   </si>
   <si>
@@ -101,6 +98,30 @@
   </si>
   <si>
     <t>Start Engine Purge Task</t>
+  </si>
+  <si>
+    <t>Ignition Sequence -Pre Tasks</t>
+  </si>
+  <si>
+    <t>Ignition Sequence - Operation</t>
+  </si>
+  <si>
+    <t>Fuel and Oxidizer Pre-Valves Open</t>
+  </si>
+  <si>
+    <t>High Pressure fluids introduced in propellant lines</t>
+  </si>
+  <si>
+    <t>MFV and MOV Open</t>
+  </si>
+  <si>
+    <t>Ethanol tapoff for Igniter</t>
+  </si>
+  <si>
+    <t>Tap-Off Line Valve Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spark Plug Start </t>
   </si>
 </sst>
 </file>
@@ -143,12 +164,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -163,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -184,6 +211,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4343CAA3-B634-E940-93C4-706CF3EA40E8}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +577,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -583,7 +611,7 @@
         <v>9</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -642,7 +670,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -736,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AE33BC-5252-A44F-9B39-E4146C0908FC}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,93 +776,238 @@
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I1" s="10"/>
+      <c r="K1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="I4" s="10"/>
+      <c r="L4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="I5" s="10"/>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I6" s="10"/>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="L7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I8" s="10"/>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I9" s="10"/>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="L10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I11" s="10"/>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I12" s="10"/>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="L13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I14" s="10"/>
+      <c r="M14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="M15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I16" s="10"/>
+      <c r="L16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L16:N16"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="L10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
controller firmware changes + doc changes (TODO -> Merge plate design)
</commit_message>
<xml_diff>
--- a/Avionics/EngineControlUnit-Firmware/Control-Module/engine tasks.xlsx
+++ b/Avionics/EngineControlUnit-Firmware/Control-Module/engine tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/EngineControlUnit-Firmware/Control-Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F354D887-4040-B249-8B3E-BEEFCFAA894F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DB55AF-4442-4E43-989F-85246B0AB7B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="27240" windowHeight="16280" activeTab="1" xr2:uid="{504D1F5D-43FB-1F42-833A-C8ADE7C72FF6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Engine Tasks</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t xml:space="preserve">Spark Plug Start </t>
+  </si>
+  <si>
+    <t>Oxidizer is passed through propeelant lines to steadily decrease pipe temps.</t>
+  </si>
+  <si>
+    <t>PID control used for process</t>
   </si>
 </sst>
 </file>
@@ -201,6 +207,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -210,8 +218,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +535,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,23 +550,23 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="H4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="O4" s="5"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -576,15 +582,15 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -599,55 +605,55 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
       <c r="I8" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
@@ -661,90 +667,95 @@
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="I12" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="J12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="J13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
+  <mergeCells count="19">
+    <mergeCell ref="J13:O13"/>
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="J9:O9"/>
     <mergeCell ref="J10:O10"/>
@@ -757,6 +768,12 @@
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="J12:O12"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -767,7 +784,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,39 +794,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="I1" s="10"/>
-      <c r="K1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="I1" s="7"/>
+      <c r="K1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I2" s="10"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="L4" s="6" t="s">
+      <c r="I4" s="7"/>
+      <c r="L4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
       <c r="O4" t="s">
         <v>21</v>
       </c>
@@ -821,7 +838,7 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="7"/>
       <c r="M5" t="s">
         <v>17</v>
       </c>
@@ -836,7 +853,7 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="7"/>
       <c r="M6" t="s">
         <v>18</v>
       </c>
@@ -845,12 +862,12 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="L7" s="6" t="s">
+      <c r="I7" s="7"/>
+      <c r="L7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -859,7 +876,7 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="7"/>
       <c r="M8" t="s">
         <v>17</v>
       </c>
@@ -868,7 +885,7 @@
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="7"/>
       <c r="M9" t="s">
         <v>18</v>
       </c>
@@ -877,12 +894,12 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="L10" s="6" t="s">
+      <c r="I10" s="7"/>
+      <c r="L10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -891,7 +908,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="7"/>
       <c r="M11" t="s">
         <v>17</v>
       </c>
@@ -900,27 +917,27 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="7"/>
       <c r="M12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="L13" s="6" t="s">
+      <c r="I13" s="7"/>
+      <c r="L13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="10"/>
+      <c r="I14" s="7"/>
       <c r="M14" t="s">
         <v>17</v>
       </c>
@@ -935,69 +952,69 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="7"/>
       <c r="M15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I16" s="10"/>
-      <c r="L16" s="6" t="s">
+      <c r="I16" s="7"/>
+      <c r="L16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="10"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" s="10"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I19" s="10"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I20" s="10"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I21" s="10"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I22" s="10"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I23" s="10"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I24" s="10"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I25" s="10"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I26" s="10"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I27" s="10"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I28" s="10"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I29" s="10"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I30" s="10"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I31" s="10"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I32" s="10"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I33" s="10"/>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>